<commit_message>
added second chance for the player, changed border block behavior, fixed and improved music integration
</commit_message>
<xml_diff>
--- a/resources/levels.xlsx
+++ b/resources/levels.xlsx
@@ -518,7 +518,7 @@
   <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -754,7 +754,7 @@
         <v>11</v>
       </c>
       <c r="G11" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="6">
         <v>1</v>

</xml_diff>